<commit_message>
Master data and user info
Master data and user info
</commit_message>
<xml_diff>
--- a/routes/Plant_001_masterdata.xlsx
+++ b/routes/Plant_001_masterdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b027ff85dd105e19/Documents/GitHub/Plant003_Nanliu Manufacturing India Private Limited/Nanliu_Manufacturing_India_Private_Limited/routes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aureo\OneDrive\Documents\GitHub\GreenInkTechnologies-SWANSON\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_379C63833E19F6E18D8ECEACF38CE0B8A079318B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC7F522-50E9-4032-A29B-6530AEA697D3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F34E1EF-9B1B-4942-8C88-4B9D31F774B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
   <si>
     <t>IRMSGCAS</t>
   </si>
@@ -73,33 +73,64 @@
     <t>Manual Typing</t>
   </si>
   <si>
-    <t>Nanliu Manufacturing India Private Limited</t>
-  </si>
-  <si>
-    <t>Sanand, Gujarat</t>
-  </si>
-  <si>
-    <t>ATBAQL 33gsm</t>
-  </si>
-  <si>
-    <t>00003768 Rev1</t>
-  </si>
-  <si>
-    <t>ATBAQL 33gsm 95mm CW NL India</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATBAQL 33gsm 90mm CW NL India</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Number_of_Slits</t>
   </si>
   <si>
-    <t>ATBAQL 40gsm</t>
+    <t>Swanson Plastics (India) Private Limited</t>
   </si>
   <si>
-    <t>AQL NL 40gsm PE/PET ATB 86mm WH</t>
+    <t>Bhuipal, Goa</t>
+  </si>
+  <si>
+    <t>APE-102(18)C</t>
+  </si>
+  <si>
+    <t>APE-168(18)C</t>
+  </si>
+  <si>
+    <t>APE-168(18)CP(KRANTI)</t>
+  </si>
+  <si>
+    <t>APE-168(18)CP(NIGHT)</t>
+  </si>
+  <si>
+    <t>APE-176(18)CP(NEEM)</t>
+  </si>
+  <si>
+    <t>WHITE-214(18)</t>
+  </si>
+  <si>
+    <t>WHITE-234(18)</t>
+  </si>
+  <si>
+    <t>99368714</t>
+  </si>
+  <si>
+    <t>00001429</t>
+  </si>
+  <si>
+    <t>99508624</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW102mmRD455mmWH BS RR</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW168mmRD400mmWH BS RR</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW168mmRD400mmWH BS RR 1CP(KRANTI)</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW168mmRD400mmWH BS RR 1CP(NIGHT)</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW176mmRD750mmWH BS RR 1CP(NEEM)</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW214mmRD510mmWH WF RR</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW234mmRD520mmWH WF RR</t>
   </si>
 </sst>
 </file>
@@ -163,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -183,21 +214,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -229,15 +245,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,41 +266,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +511,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O999"/>
+  <dimension ref="A1:O997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -514,8 +522,9 @@
     <col min="1" max="1" width="14.42578125" style="1"/>
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" style="1" customWidth="1"/>
@@ -539,7 +548,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -566,31 +575,31 @@
       <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>23</v>
+      <c r="N1" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="8">
-        <v>90109685</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="2" spans="1:15" s="13" customFormat="1" ht="15">
+      <c r="A2" s="9">
+        <v>99396168</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>21</v>
+      <c r="E2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>14</v>
@@ -598,8 +607,8 @@
       <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="8">
-        <v>95</v>
+      <c r="I2" s="12">
+        <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>16</v>
@@ -621,23 +630,23 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="8">
-        <v>90252662</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="1">
+        <v>91876235</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>22</v>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>14</v>
@@ -645,8 +654,8 @@
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="8">
-        <v>90</v>
+      <c r="I3" s="1">
+        <v>168</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>16</v>
@@ -667,24 +676,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="20" customFormat="1" ht="15">
-      <c r="A4" s="14">
-        <v>90415042</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="16" t="s">
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="1">
+        <v>90254197</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>25</v>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>14</v>
@@ -692,8 +701,8 @@
       <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="17">
-        <v>86</v>
+      <c r="I4" s="1">
+        <v>168</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>16</v>
@@ -714,44 +723,212 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12.75">
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" ht="12.75">
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="12.75">
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" ht="12.75">
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" ht="12.75">
+    <row r="5" spans="1:15" ht="15">
+      <c r="A5" s="1">
+        <v>90486174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1">
+        <v>168</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15">
+      <c r="A6" s="1">
+        <v>90256104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1">
+        <v>176</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15">
+      <c r="A7" s="1">
+        <v>91000940</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1">
+        <v>214</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15">
+      <c r="A8" s="1">
+        <v>96977186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1">
+        <v>234</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="12.75">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="12.75">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:15" ht="12.75">
       <c r="F10" s="7"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="12.75">
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
+    </row>
+    <row r="11" spans="1:15" ht="12.75">
       <c r="F11" s="7"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="N11"/>
     </row>
     <row r="12" spans="1:15" ht="12.75">
       <c r="F12" s="7"/>
@@ -3675,12 +3852,8 @@
     <row r="985" spans="6:6" ht="12.75">
       <c r="F985" s="7"/>
     </row>
-    <row r="986" spans="6:6" ht="12.75">
-      <c r="F986" s="7"/>
-    </row>
-    <row r="987" spans="6:6" ht="12.75">
-      <c r="F987" s="7"/>
-    </row>
+    <row r="986" spans="6:6" ht="12.75"/>
+    <row r="987" spans="6:6" ht="12.75"/>
     <row r="988" spans="6:6" ht="12.75"/>
     <row r="989" spans="6:6" ht="12.75"/>
     <row r="990" spans="6:6" ht="12.75"/>
@@ -3691,8 +3864,6 @@
     <row r="995" ht="12.75"/>
     <row r="996" ht="12.75"/>
     <row r="997" ht="12.75"/>
-    <row r="998" ht="12.75"/>
-    <row r="999" ht="12.75"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pallet number and PI
Pallet number and PI
</commit_message>
<xml_diff>
--- a/routes/Plant_001_masterdata.xlsx
+++ b/routes/Plant_001_masterdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aureo\OneDrive\Documents\GitHub\GreenInkTechnologies-SWANSON\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F34E1EF-9B1B-4942-8C88-4B9D31F774B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B3552C-262A-4097-B48F-F26C07B57C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t>IRMSGCAS</t>
   </si>
@@ -131,13 +131,25 @@
   </si>
   <si>
     <t>FI SWA 18gsm CW234mmRD520mmWH WF RR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI Number </t>
+  </si>
+  <si>
+    <t>UBS23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pallet Number </t>
+  </si>
+  <si>
+    <t>Std WT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,6 +185,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -194,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -226,26 +249,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -267,32 +275,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +532,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O997"/>
+  <dimension ref="A1:R997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="O13" sqref="O13:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -523,7 +544,7 @@
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="56.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
@@ -533,9 +554,10 @@
     <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
     <col min="15" max="15" width="26" style="1" customWidth="1"/>
+    <col min="16" max="18" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="12.75">
+    <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +570,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -581,24 +603,33 @@
       <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="13" customFormat="1" ht="15">
-      <c r="A2" s="9">
+      <c r="P1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="9" customFormat="1" ht="15">
+      <c r="A2" s="14">
         <v>99396168</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -607,7 +638,7 @@
       <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="18">
         <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -628,24 +659,31 @@
       <c r="O2" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="1">
+      <c r="P2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="14"/>
+    </row>
+    <row r="3" spans="1:18" ht="15">
+      <c r="A3" s="14">
         <v>91876235</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="23" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -654,7 +692,7 @@
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="14">
         <v>168</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -675,24 +713,33 @@
       <c r="O3" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="1">
+      <c r="P3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="14">
+        <v>14.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15">
+      <c r="A4" s="14">
         <v>90254197</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -701,7 +748,7 @@
       <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="14">
         <v>168</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -722,24 +769,33 @@
       <c r="O4" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15">
-      <c r="A5" s="1">
+      <c r="P4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="14">
+        <v>14.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15">
+      <c r="A5" s="14">
         <v>90486174</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="23" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -748,7 +804,7 @@
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="14">
         <v>168</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -769,24 +825,31 @@
       <c r="O5" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15">
-      <c r="A6" s="1">
+      <c r="P5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" ht="15">
+      <c r="A6" s="14">
         <v>90256104</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="23" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -795,7 +858,7 @@
       <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="14">
         <v>176</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -816,24 +879,31 @@
       <c r="O6" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15">
-      <c r="A7" s="1">
+      <c r="P6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" ht="15">
+      <c r="A7" s="14">
         <v>91000940</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="23" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -842,7 +912,7 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="14">
         <v>214</v>
       </c>
       <c r="J7" s="6" t="s">
@@ -863,24 +933,33 @@
       <c r="O7" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15">
-      <c r="A8" s="1">
+      <c r="P7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="14">
+        <v>25.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="1" customFormat="1" ht="15">
+      <c r="A8" s="14">
         <v>96977186</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="23" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -889,7 +968,7 @@
       <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="14">
         <v>234</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -910,12 +989,19 @@
       <c r="O8" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="12.75">
+      <c r="P8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" s="1" customFormat="1" ht="12.75">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -924,25 +1010,25 @@
       <c r="L9"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:15" ht="12.75">
+    <row r="10" spans="1:18" ht="12.75">
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:15" ht="12.75">
+    <row r="11" spans="1:18" ht="12.75">
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:15" ht="12.75">
+    <row r="12" spans="1:18" ht="12.75">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:15" ht="12.75">
+    <row r="13" spans="1:18" ht="12.75">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:15" ht="12.75">
+    <row r="14" spans="1:18" ht="12.75">
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="12.75">
+    <row r="15" spans="1:18" ht="12.75">
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:15" ht="12.75">
+    <row r="16" spans="1:18" ht="12.75">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="6:6" ht="12.75">

</xml_diff>

<commit_message>
New CR from P&G from goa
New CR from P&G from goa
</commit_message>
<xml_diff>
--- a/routes/Plant_001_masterdata.xlsx
+++ b/routes/Plant_001_masterdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aureo\OneDrive\Documents\GitHub\GreenInkTechnologies-SWANSON\GreenInkTechnologies-SWANSON\routes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aureoleinc-my.sharepoint.com/personal/suraj_patil_vegam_co/Documents/Documents/GitHub/GreenInkTechnologies-SWANSON/routes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AE9A56-8872-4CC4-BBCB-10AFAE46FAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{07AE9A56-8872-4CC4-BBCB-10AFAE46FAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FC35007-A8CF-4922-B6B8-2050B20FFF7D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
   <si>
     <t>IRMSGCAS</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>FI SWA 18gsm CW176mmRD750mmWH BS RR 1CP FGC (NEEM)</t>
+  </si>
+  <si>
+    <t>00003055</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW168mmRD415mmWH BS RR</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -354,6 +360,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -577,7 +590,7 @@
   <dimension ref="A1:S997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1132,8 +1145,64 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="12.75">
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:19" ht="15">
+      <c r="A10" s="30">
+        <v>91899840</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="30">
+        <v>168</v>
+      </c>
+      <c r="J10" s="30">
+        <v>14.21</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="29">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:19" ht="12.75">
       <c r="F11" s="7"/>

</xml_diff>

<commit_message>
material and new user added
</commit_message>
<xml_diff>
--- a/routes/Plant_001_masterdata.xlsx
+++ b/routes/Plant_001_masterdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aureoleinc-my.sharepoint.com/personal/suraj_patil_vegam_co/Documents/Documents/GitHub/GreenInkTechnologies-SWANSON_latest/GreenInkTechnologies-SWANSON/routes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aureoleinc-my.sharepoint.com/personal/suraj_patil_vegam_co/Documents/Documents/GitHub/GreenInkTechnologies-SWANSON_v2/GreenInkTechnologies-SWANSON/routes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{07AE9A56-8872-4CC4-BBCB-10AFAE46FAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CA541FA-B245-4B3C-8010-499B2719EF70}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{07AE9A56-8872-4CC4-BBCB-10AFAE46FAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605E33A4-18FA-4DBA-A196-0D322A9D10AF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="49">
   <si>
     <t>IRMSGCAS</t>
   </si>
@@ -151,9 +151,6 @@
     <t>APE-176(18)CP(FGC-NEEM)</t>
   </si>
   <si>
-    <t>FI SWA 18gsm CW176mmRD750mmWH BS RR 1CP FGC (NEEM)</t>
-  </si>
-  <si>
     <t>00003055</t>
   </si>
   <si>
@@ -163,7 +160,13 @@
     <t>APE-176(18)CP(EASY JET)</t>
   </si>
   <si>
-    <t>FI SWA 18gsm CW176mmRD650mmWH BS RR 1CP(EASY JET)</t>
+    <t>00004986</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW176mmRD740mmWH BS RR 1CP FGC (NEEM)</t>
+  </si>
+  <si>
+    <t>FI SWA 18gsm CW176mmRD740mmWH BS RR 1CP(EASY JET)</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -615,8 +614,8 @@
   </sheetPr>
   <dimension ref="A1:S997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -626,7 +625,7 @@
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="56.42578125" customWidth="1"/>
+    <col min="6" max="6" width="62.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" style="1" customWidth="1"/>
@@ -935,7 +934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="14">
         <v>90256104</v>
       </c>
@@ -949,10 +948,10 @@
         <v>42</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>14</v>
@@ -1185,10 +1184,10 @@
         <v>21</v>
       </c>
       <c r="E10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>45</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>14</v>
@@ -1241,13 +1240,13 @@
         <v>19</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>27</v>
-      </c>
       <c r="F11" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>14</v>

</xml_diff>